<commit_message>
Added filtering to DC link current measurement, also included D part in power calculation. Added PWM input measurement, will have to ckeck if it works and add timeout checking.
</commit_message>
<xml_diff>
--- a/ebaesc_sw/documents/Preizkusi.xlsx
+++ b/ebaesc_sw/documents/Preizkusi.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="0,05" sheetId="2" r:id="rId2"/>
     <sheet name="0,1" sheetId="3" r:id="rId3"/>
+    <sheet name="0,1_1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="33">
   <si>
     <t>Umax</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>eff</t>
+  </si>
+  <si>
+    <t>Pin(Q)</t>
   </si>
 </sst>
 </file>
@@ -2123,7 +2127,7 @@
   <dimension ref="A2:Y18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2841,20 +2845,20 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <f>I13+S13</f>
-        <v>64.000178880000007</v>
+        <f>I14+S14</f>
+        <v>73.453499999999991</v>
       </c>
       <c r="K16">
-        <f>K13+U13</f>
-        <v>63.257857056000063</v>
+        <f t="shared" ref="J16:O16" si="1">K14+U14</f>
+        <v>82.466000000000037</v>
       </c>
       <c r="M16">
-        <f>M13+W13</f>
-        <v>58.583235839999986</v>
+        <f t="shared" si="1"/>
+        <v>69.149129999999985</v>
       </c>
       <c r="O16">
-        <f>O13+Y13</f>
-        <v>79.849752959999989</v>
+        <f t="shared" si="1"/>
+        <v>128.06074000000001</v>
       </c>
     </row>
     <row r="18" spans="7:15" x14ac:dyDescent="0.25">
@@ -2862,20 +2866,20 @@
         <v>31</v>
       </c>
       <c r="I18">
-        <f>1-((I16/2)/I13)</f>
-        <v>0.76158445440956646</v>
+        <f>1-((I16/2)/I14)</f>
+        <v>0.72661954846921684</v>
       </c>
       <c r="K18">
-        <f>1-((K16/2)/K13)</f>
-        <v>0.85553926509667355</v>
+        <f t="shared" ref="J18:O18" si="2">1-((K16/2)/K14)</f>
+        <v>0.82877229992359047</v>
       </c>
       <c r="M18">
-        <f>1-((M16/2)/M13)</f>
-        <v>0.90214477211796251</v>
+        <f t="shared" si="2"/>
+        <v>0.88849791989164084</v>
       </c>
       <c r="O18">
-        <f>1-((O16/2)/O13)</f>
-        <v>0.87924757281553401</v>
+        <f t="shared" si="2"/>
+        <v>0.81523163003832122</v>
       </c>
     </row>
   </sheetData>
@@ -2887,8 +2891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,4 +3770,910 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Y23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>60.87</v>
+      </c>
+      <c r="I2">
+        <v>164.8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2">
+        <v>60.87</v>
+      </c>
+      <c r="S2">
+        <v>164.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="J3">
+        <v>0.2</v>
+      </c>
+      <c r="L3">
+        <v>0.3</v>
+      </c>
+      <c r="N3">
+        <v>0.4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3">
+        <v>0.1</v>
+      </c>
+      <c r="T3">
+        <v>0.2</v>
+      </c>
+      <c r="V3">
+        <v>0.3</v>
+      </c>
+      <c r="X3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="11">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11">
+        <v>19</v>
+      </c>
+      <c r="D4" s="11">
+        <v>19</v>
+      </c>
+      <c r="E4" s="11">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="11">
+        <v>-0.04</v>
+      </c>
+      <c r="I4" s="12">
+        <f>H4*H2</f>
+        <v>-2.4348000000000001</v>
+      </c>
+      <c r="J4" s="11">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="K4" s="12">
+        <f>J4*H2</f>
+        <v>-6.2087399999999997</v>
+      </c>
+      <c r="L4" s="11">
+        <v>-0.23400000000000001</v>
+      </c>
+      <c r="M4" s="12">
+        <f>L4*H2</f>
+        <v>-14.24358</v>
+      </c>
+      <c r="N4" s="11">
+        <v>-0.22900000000000001</v>
+      </c>
+      <c r="O4" s="12">
+        <f>N4*H2</f>
+        <v>-13.93923</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0</v>
+      </c>
+      <c r="S4" s="12">
+        <f>R4*R2</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="11">
+        <v>0</v>
+      </c>
+      <c r="U4" s="12">
+        <f>T4*R2</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="11">
+        <v>0</v>
+      </c>
+      <c r="W4" s="12">
+        <f>V4*R2</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="12">
+        <f>X4*R2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="11">
+        <v>4.3</v>
+      </c>
+      <c r="C5" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D5" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>6.8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="I5" s="12">
+        <f>H5*H2</f>
+        <v>18.078389999999999</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="K5" s="12">
+        <f>J5*H2</f>
+        <v>29.278469999999999</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="M5" s="12">
+        <f>L5*H2</f>
+        <v>44.982929999999996</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="O5" s="12">
+        <f>N5*H2</f>
+        <v>50.765579999999993</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="11">
+        <v>-0.108</v>
+      </c>
+      <c r="S5" s="12">
+        <f>R5*R2</f>
+        <v>-6.5739599999999996</v>
+      </c>
+      <c r="T5" s="11">
+        <v>-0.248</v>
+      </c>
+      <c r="U5" s="12">
+        <f>T5*R2</f>
+        <v>-15.095759999999999</v>
+      </c>
+      <c r="V5" s="11">
+        <v>-0.43099999999999999</v>
+      </c>
+      <c r="W5" s="12">
+        <f>V5*R2</f>
+        <v>-26.234969999999997</v>
+      </c>
+      <c r="X5" s="11">
+        <v>-0.66400000000000003</v>
+      </c>
+      <c r="Y5" s="12">
+        <f>X5*R2</f>
+        <v>-40.417679999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="12">
+        <f>B5*B4</f>
+        <v>81.7</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" ref="C6:E6" si="0">C5*C4</f>
+        <v>96.899999999999991</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>110.2</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" si="0"/>
+        <v>129.19999999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <f>H6*I2</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <f>J6*I2</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M6" s="12">
+        <f>L6*I2</f>
+        <v>2.8016000000000005</v>
+      </c>
+      <c r="N6" s="11">
+        <v>-0.01</v>
+      </c>
+      <c r="O6" s="12">
+        <f>N6*I2</f>
+        <v>-1.6480000000000001</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12">
+        <f>R6*S2</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="11">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12">
+        <f>T6*S2</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="11">
+        <v>0</v>
+      </c>
+      <c r="W6" s="12">
+        <f>V6*S2</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="12">
+        <f>X6*S2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="12">
+        <f>H7*I2</f>
+        <v>16.48</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="12">
+        <f>J7*I2</f>
+        <v>16.48</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="M7" s="12">
+        <f>L7*I2</f>
+        <v>16.48</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="12">
+        <f>N7*I2</f>
+        <v>16.48</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="S7" s="12">
+        <f>R7*S2</f>
+        <v>16.48</v>
+      </c>
+      <c r="T7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="U7" s="12">
+        <f>T7*S2</f>
+        <v>16.48</v>
+      </c>
+      <c r="V7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="W7" s="12">
+        <f>V7*S2</f>
+        <v>16.48</v>
+      </c>
+      <c r="X7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="Y7" s="12">
+        <f>X7*S2</f>
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="11">
+        <v>8.1</v>
+      </c>
+      <c r="I8" s="12">
+        <f>H8</f>
+        <v>8.1</v>
+      </c>
+      <c r="J8" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="K8" s="12">
+        <f>J8</f>
+        <v>13.5</v>
+      </c>
+      <c r="L8" s="11">
+        <v>17.2</v>
+      </c>
+      <c r="M8" s="12">
+        <f>L8</f>
+        <v>17.2</v>
+      </c>
+      <c r="N8" s="11">
+        <v>20.3</v>
+      </c>
+      <c r="O8" s="12">
+        <f>N8</f>
+        <v>20.3</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="S8" s="12">
+        <f>R8</f>
+        <v>-2.5</v>
+      </c>
+      <c r="T8" s="11">
+        <v>-7.17</v>
+      </c>
+      <c r="U8" s="12">
+        <f>T8</f>
+        <v>-7.17</v>
+      </c>
+      <c r="V8" s="11">
+        <v>-9.9</v>
+      </c>
+      <c r="W8" s="12">
+        <f>V8</f>
+        <v>-9.9</v>
+      </c>
+      <c r="X8" s="11">
+        <v>-13.4</v>
+      </c>
+      <c r="Y8" s="12">
+        <f>X8</f>
+        <v>-13.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="11">
+        <v>18.7</v>
+      </c>
+      <c r="I9" s="12">
+        <f>H9</f>
+        <v>18.7</v>
+      </c>
+      <c r="J9" s="11">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K9" s="12">
+        <f>J9</f>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="L9" s="11">
+        <v>18.55</v>
+      </c>
+      <c r="M9" s="12">
+        <f>L9</f>
+        <v>18.55</v>
+      </c>
+      <c r="N9" s="11">
+        <v>18.440000000000001</v>
+      </c>
+      <c r="O9" s="12">
+        <f>N9</f>
+        <v>18.440000000000001</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="11">
+        <v>18.63</v>
+      </c>
+      <c r="S9" s="12">
+        <f>R9</f>
+        <v>18.63</v>
+      </c>
+      <c r="T9" s="11">
+        <v>18.63</v>
+      </c>
+      <c r="U9" s="12">
+        <f>T9</f>
+        <v>18.63</v>
+      </c>
+      <c r="V9" s="11">
+        <v>18.63</v>
+      </c>
+      <c r="W9" s="12">
+        <f>V9</f>
+        <v>18.63</v>
+      </c>
+      <c r="X9" s="11">
+        <v>18.63</v>
+      </c>
+      <c r="Y9" s="12">
+        <f>X9</f>
+        <v>18.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="11">
+        <v>153</v>
+      </c>
+      <c r="I10" s="12">
+        <f>H10</f>
+        <v>153</v>
+      </c>
+      <c r="J10" s="11">
+        <v>231</v>
+      </c>
+      <c r="K10" s="12">
+        <f>J10</f>
+        <v>231</v>
+      </c>
+      <c r="L10" s="11">
+        <v>350</v>
+      </c>
+      <c r="M10" s="12">
+        <f>L10</f>
+        <v>350</v>
+      </c>
+      <c r="N10" s="11">
+        <v>426</v>
+      </c>
+      <c r="O10" s="12">
+        <f>N10</f>
+        <v>426</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="11">
+        <v>-47</v>
+      </c>
+      <c r="S10" s="12">
+        <f>R10</f>
+        <v>-47</v>
+      </c>
+      <c r="T10" s="11">
+        <v>-133</v>
+      </c>
+      <c r="U10" s="12">
+        <f>T10</f>
+        <v>-133</v>
+      </c>
+      <c r="V10" s="11">
+        <v>-176</v>
+      </c>
+      <c r="W10" s="12">
+        <f>V10</f>
+        <v>-176</v>
+      </c>
+      <c r="X10" s="11">
+        <v>-250</v>
+      </c>
+      <c r="Y10" s="12">
+        <f>X10</f>
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1700</v>
+      </c>
+      <c r="I11" s="12">
+        <f>H11</f>
+        <v>1700</v>
+      </c>
+      <c r="J11" s="11">
+        <v>3400</v>
+      </c>
+      <c r="K11" s="12">
+        <f>J11</f>
+        <v>3400</v>
+      </c>
+      <c r="L11" s="11">
+        <v>5150</v>
+      </c>
+      <c r="M11" s="12">
+        <f>L11</f>
+        <v>5150</v>
+      </c>
+      <c r="N11" s="11">
+        <v>6900</v>
+      </c>
+      <c r="O11" s="12">
+        <f>N11</f>
+        <v>6900</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>25</v>
+      </c>
+      <c r="R11" s="11">
+        <v>1700</v>
+      </c>
+      <c r="S11" s="12">
+        <f>R11</f>
+        <v>1700</v>
+      </c>
+      <c r="T11" s="11">
+        <v>3400</v>
+      </c>
+      <c r="U11" s="12">
+        <f>T11</f>
+        <v>3400</v>
+      </c>
+      <c r="V11" s="11">
+        <v>5150</v>
+      </c>
+      <c r="W11" s="12">
+        <f>V11</f>
+        <v>5150</v>
+      </c>
+      <c r="X11" s="11">
+        <v>6900</v>
+      </c>
+      <c r="Y11" s="12">
+        <f>X11</f>
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13">
+        <f>(I4*I6+I5*I7)</f>
+        <v>297.9318672</v>
+      </c>
+      <c r="K13">
+        <f>(K4*K6+K5*K7)</f>
+        <v>482.50918559999997</v>
+      </c>
+      <c r="M13">
+        <f>(M4*M6+M5*M7)</f>
+        <v>701.41387267199991</v>
+      </c>
+      <c r="O13">
+        <f>(O4*O6+O5*O7)</f>
+        <v>859.58860943999991</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13">
+        <f>(S4*S6+S5*S7)</f>
+        <v>-108.33886079999999</v>
+      </c>
+      <c r="U13">
+        <f>(U4*U6+U5*U7)</f>
+        <v>-248.77812479999997</v>
+      </c>
+      <c r="W13">
+        <f>(W4*W6+W5*W7)</f>
+        <v>-432.35230559999997</v>
+      </c>
+      <c r="Y13">
+        <f>(Y4*Y6+Y5*Y7)</f>
+        <v>-666.08336639999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <f>I5*I7</f>
+        <v>297.9318672</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="J14:O14" si="1">K5*K7</f>
+        <v>482.50918559999997</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>741.31868639999993</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>836.61675839999987</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15">
+        <f>I8*I9</f>
+        <v>151.47</v>
+      </c>
+      <c r="K15">
+        <f>K8*K9</f>
+        <v>251.10000000000002</v>
+      </c>
+      <c r="M15">
+        <f>M8*M9</f>
+        <v>319.06</v>
+      </c>
+      <c r="O15">
+        <f>O8*O9</f>
+        <v>374.33200000000005</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15">
+        <f>S8*S9</f>
+        <v>-46.574999999999996</v>
+      </c>
+      <c r="U15">
+        <f>U8*U9</f>
+        <v>-133.5771</v>
+      </c>
+      <c r="W15">
+        <f>W8*W9</f>
+        <v>-184.43699999999998</v>
+      </c>
+      <c r="Y15">
+        <f>Y8*Y9</f>
+        <v>-249.642</v>
+      </c>
+    </row>
+    <row r="17" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <f>SQRT(I4^2+I5^2)</f>
+        <v>18.241612758528234</v>
+      </c>
+      <c r="K17">
+        <f>SQRT(K4^2+K5^2)</f>
+        <v>29.929538217762396</v>
+      </c>
+      <c r="M17">
+        <f>SQRT(M4^2+M5^2)</f>
+        <v>47.18414524606014</v>
+      </c>
+      <c r="O17">
+        <f>SQRT(O4^2+O5^2)</f>
+        <v>52.644527215364938</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S17">
+        <f>SQRT(S4^2+S5^2)</f>
+        <v>6.5739599999999996</v>
+      </c>
+      <c r="U17">
+        <f>SQRT(U4^2+U5^2)</f>
+        <v>15.095759999999999</v>
+      </c>
+      <c r="W17">
+        <f>SQRT(W4^2+W5^2)</f>
+        <v>26.234969999999997</v>
+      </c>
+      <c r="Y17">
+        <f>SQRT(Y4^2+Y5^2)</f>
+        <v>40.417679999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <f>SQRT(I6^2+I7^2)</f>
+        <v>16.48</v>
+      </c>
+      <c r="K18">
+        <f>SQRT(K6^2+K7^2)</f>
+        <v>16.48</v>
+      </c>
+      <c r="M18">
+        <f>SQRT(M6^2+M7^2)</f>
+        <v>16.71643988892372</v>
+      </c>
+      <c r="O18">
+        <f>SQRT(O6^2+O7^2)</f>
+        <v>16.562195023607227</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>13</v>
+      </c>
+      <c r="S18">
+        <f>SQRT(S6^2+S7^2)</f>
+        <v>16.48</v>
+      </c>
+      <c r="U18">
+        <f>SQRT(U6^2+U7^2)</f>
+        <v>16.48</v>
+      </c>
+      <c r="W18">
+        <f>SQRT(W6^2+W7^2)</f>
+        <v>16.48</v>
+      </c>
+      <c r="Y18">
+        <f>SQRT(Y6^2+Y7^2)</f>
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="19" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <f>I17*I18</f>
+        <v>300.62177826054528</v>
+      </c>
+      <c r="K19">
+        <f>K17*K18</f>
+        <v>493.23878982872429</v>
+      </c>
+      <c r="M19">
+        <f>M17*M18</f>
+        <v>788.75092771601021</v>
+      </c>
+      <c r="O19">
+        <f>O17*O18</f>
+        <v>871.90892666647244</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S19">
+        <f>S17*S18</f>
+        <v>108.33886079999999</v>
+      </c>
+      <c r="U19">
+        <f>U17*U18</f>
+        <v>248.77812479999997</v>
+      </c>
+      <c r="W19">
+        <f>W17*W18</f>
+        <v>432.35230559999997</v>
+      </c>
+      <c r="Y19">
+        <f>Y17*Y18</f>
+        <v>666.08336639999993</v>
+      </c>
+    </row>
+    <row r="21" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <f>I15+S15</f>
+        <v>104.89500000000001</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:O21" si="2">K15+U15</f>
+        <v>117.52290000000002</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>134.62300000000002</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>124.69000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23">
+        <f>1-((I21/2)/I15)</f>
+        <v>0.65374331550802134</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23:O23" si="3">1-((K21/2)/K15)</f>
+        <v>0.7659838709677419</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>0.7890318435403999</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="3"/>
+        <v>0.83344998557430294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>